<commit_message>
Add HowAppWorksPopupPage, HomePage updates, and related tests
- Added HowAppWorksPopupPage with Step 1 verification methods
- Updated HomePage with Let's Go banner click and text verification
- Added test cases for banner text, popup open validation, and Step 1 checks
- Integrated data-driven assertions using ExcelUtils
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>UIElement</t>
   </si>
@@ -20,6 +20,48 @@
   </si>
   <si>
     <t>splashText</t>
+  </si>
+  <si>
+    <t>ShortLocation</t>
+  </si>
+  <si>
+    <t>5 Empress Pl</t>
+  </si>
+  <si>
+    <t>FullLocation</t>
+  </si>
+  <si>
+    <t>5 Empress Pl, Singapore</t>
+  </si>
+  <si>
+    <t>YourWallets</t>
+  </si>
+  <si>
+    <t>Your Wallets</t>
+  </si>
+  <si>
+    <t>HowAppWorksBanner</t>
+  </si>
+  <si>
+    <t>Let's Go!</t>
+  </si>
+  <si>
+    <t>Step1Title</t>
+  </si>
+  <si>
+    <t>Step 1</t>
+  </si>
+  <si>
+    <t>Step1DescTitle</t>
+  </si>
+  <si>
+    <t>Find an offer</t>
+  </si>
+  <si>
+    <t>Step1DescDetail</t>
+  </si>
+  <si>
+    <t>Upto 40% credits up for grabs! Keep a lookout!</t>
   </si>
 </sst>
 </file>
@@ -277,7 +319,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="25.88"/>
-    <col customWidth="1" min="2" max="2" width="30.38"/>
+    <col customWidth="1" min="2" max="2" width="59.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -295,8 +337,60 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>